<commit_message>
Check For Existing Tables When Collecting
</commit_message>
<xml_diff>
--- a/tests/temperature-table.xlsx
+++ b/tests/temperature-table.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\rust\calamine\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\williamcarroll\Projects\rust\calamine\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6E38F2-295A-4860-810F-AD0B70BB07E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F17DC-FC8A-4ADC-A329-46504DBE5193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="3670" windowWidth="35640" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38010" yWindow="390" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>label</t>
   </si>
@@ -32,6 +33,18 @@
   </si>
   <si>
     <t>fahrenheit</t>
+  </si>
+  <si>
+    <t>something</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>label2</t>
+  </si>
+  <si>
+    <t>value2</t>
   </si>
 </sst>
 </file>
@@ -83,7 +96,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -120,8 +152,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{437B11C6-D742-458D-B86A-3EC8718A1854}" name="Temperature" displayName="Temperature" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3" xr:uid="{1B8C896A-B06E-4FF4-9465-348B6F9418BE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{548E04E2-5CD2-4DDF-B944-9559DB726EC5}" name="label" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{548E04E2-5CD2-4DDF-B944-9559DB726EC5}" name="label" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{859B4355-0FDA-4406-B967-637A8E88A9BF}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7CC8FB0B-5F4D-4E9C-8F2B-CF28A0E2E1FD}" name="OtherTable" displayName="OtherTable" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{8EF8620A-1981-4FB1-8512-C8EFBE89560D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{87892161-2992-47E3-AD53-CC40B8D85ED9}" name="label2" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{47B8E2C3-5419-4D70-A2FE-0AF4B60B1B9B}" name="value2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -426,11 +469,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -454,6 +497,48 @@
       </c>
       <c r="B3" s="1">
         <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DED292-7494-4549-B8B9-E3B8845566FD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>